<commit_message>
Fix for double-search on new game
</commit_message>
<xml_diff>
--- a/Project1/Project1/Project1.xlsx
+++ b/Project1/Project1/Project1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="27280" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="27280" windowHeight="16260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BFS Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="174">
   <si>
     <t>BFS</t>
   </si>
@@ -42,526 +42,514 @@
     <t>Memory(MB)</t>
   </si>
   <si>
+    <t xml:space="preserve">4 _ 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 8 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 7 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 _ 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 _ 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 2 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 2 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 6 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 _ 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 5 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 5 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 _ 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 5 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 _ 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 8 _ </t>
+  </si>
+  <si>
+    <t>Boards Examined</t>
+  </si>
+  <si>
+    <t>Move 1</t>
+  </si>
+  <si>
+    <t>Move 2</t>
+  </si>
+  <si>
+    <t>Move 3</t>
+  </si>
+  <si>
+    <t>Move 4</t>
+  </si>
+  <si>
+    <t>Move 5</t>
+  </si>
+  <si>
+    <t>Move 6</t>
+  </si>
+  <si>
+    <t>Move 7</t>
+  </si>
+  <si>
+    <t>Move 8</t>
+  </si>
+  <si>
+    <t>Move 9</t>
+  </si>
+  <si>
+    <t>Move 10</t>
+  </si>
+  <si>
+    <t>Move 11</t>
+  </si>
+  <si>
+    <t>Move 12</t>
+  </si>
+  <si>
+    <t>Move 13</t>
+  </si>
+  <si>
+    <t>Move 14</t>
+  </si>
+  <si>
+    <t>Move 15</t>
+  </si>
+  <si>
+    <t>Move 16</t>
+  </si>
+  <si>
+    <t>Move 17</t>
+  </si>
+  <si>
+    <t>Move 18</t>
+  </si>
+  <si>
+    <t>Move 19</t>
+  </si>
+  <si>
+    <t>Move 20</t>
+  </si>
+  <si>
+    <t>Move 21</t>
+  </si>
+  <si>
+    <t>Move 22</t>
+  </si>
+  <si>
+    <t>Move 23</t>
+  </si>
+  <si>
+    <t>Move 24</t>
+  </si>
+  <si>
+    <t>Move 25</t>
+  </si>
+  <si>
+    <t>Move 26</t>
+  </si>
+  <si>
+    <t>Move 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 _ 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 1 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 _ 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 5 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 8 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 _ 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 5 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 2 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 5 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 _ 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 _ 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 7 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 4 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 _ 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 1 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 7 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 _ 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 3 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 1 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 3 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 _ 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 7 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 7 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 _ 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 8 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 _ 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 1 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 7 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 4 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 _ 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 5 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 _ 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 5 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 1 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 5 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 _ 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 5 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 _ 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 7 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 1 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 8 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 1 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 1 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 _ 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 4 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 _ 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 8 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 6 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 _ 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 _ 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 2 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 1 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 5 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 5 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 _ 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 2 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 5 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 2 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 1 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 _ 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 5 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 2 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 2 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 6 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 4 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 4 2 </t>
+  </si>
+  <si>
+    <t>Approx Time(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 3 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 8 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 5 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 8 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 5 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 _ 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 _ 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 8 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 2 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 3 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 2 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 2 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 2 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 7 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 7 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 1 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 6 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 7 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 1 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 1 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 _ 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 2 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 2 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 2 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 8 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 8 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 6 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 _ 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 4 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 7 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 1 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 7 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 _ 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 7 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 1 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 2 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 8 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 8 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 5 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 7 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 1 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 _ 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 7 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 _ 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 5 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ 7 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 _ 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 5 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 8 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 3 _ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 8 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 1 5 </t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>StdDev</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>Boards</t>
+  </si>
+  <si>
     <t>SOLVED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 _ 7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 8 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 7 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 _ 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 _ 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 2 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 2 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 6 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 _ 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 5 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 5 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 _ 6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 5 6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 _ 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 8 _ </t>
-  </si>
-  <si>
-    <t>Boards Examined</t>
-  </si>
-  <si>
-    <t>Move 1</t>
-  </si>
-  <si>
-    <t>Move 2</t>
-  </si>
-  <si>
-    <t>Move 3</t>
-  </si>
-  <si>
-    <t>Move 4</t>
-  </si>
-  <si>
-    <t>Move 5</t>
-  </si>
-  <si>
-    <t>Move 6</t>
-  </si>
-  <si>
-    <t>Move 7</t>
-  </si>
-  <si>
-    <t>Move 8</t>
-  </si>
-  <si>
-    <t>Move 9</t>
-  </si>
-  <si>
-    <t>Move 10</t>
-  </si>
-  <si>
-    <t>Move 11</t>
-  </si>
-  <si>
-    <t>Move 12</t>
-  </si>
-  <si>
-    <t>Move 13</t>
-  </si>
-  <si>
-    <t>Move 14</t>
-  </si>
-  <si>
-    <t>Move 15</t>
-  </si>
-  <si>
-    <t>Move 16</t>
-  </si>
-  <si>
-    <t>Move 17</t>
-  </si>
-  <si>
-    <t>Move 18</t>
-  </si>
-  <si>
-    <t>Move 19</t>
-  </si>
-  <si>
-    <t>Move 20</t>
-  </si>
-  <si>
-    <t>Move 21</t>
-  </si>
-  <si>
-    <t>Move 22</t>
-  </si>
-  <si>
-    <t>Move 23</t>
-  </si>
-  <si>
-    <t>Move 24</t>
-  </si>
-  <si>
-    <t>Move 25</t>
-  </si>
-  <si>
-    <t>Move 26</t>
-  </si>
-  <si>
-    <t>Move 27</t>
-  </si>
-  <si>
-    <t>Move 28</t>
-  </si>
-  <si>
-    <t>Move 29</t>
-  </si>
-  <si>
-    <t>Move 30</t>
-  </si>
-  <si>
-    <t>Move 31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 _ 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 1 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 _ 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 5 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 8 6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 _ 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 5 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 2 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 5 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 _ 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 _ 6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 7 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 4 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 _ 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 1 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 7 6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 _ 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 3 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 1 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 3 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 _ 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 7 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 7 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 _ 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 8 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 _ 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 1 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 7 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 4 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 _ 7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 5 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 _ 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 5 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 1 7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 5 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 _ 7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 5 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 _ 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 7 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 1 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 8 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 1 7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 1 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 _ 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 4 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 _ 7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 8 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 6 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 _ 6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 _ 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 2 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 1 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 5 6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 5 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 _ 6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 2 6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 5 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 2 6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 1 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 _ 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 5 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 2 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 2 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 6 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 4 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 4 2 </t>
-  </si>
-  <si>
-    <t>Approx Time(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 3 7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 8 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 5 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 8 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 5 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 _ 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 _ 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 8 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 2 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 3 7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 2 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 2 7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 2 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 7 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 7 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 1 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 6 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 7 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 1 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 1 7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 _ 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 2 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 2 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 2 7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 8 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 8 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 6 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 _ 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 4 7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 7 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 1 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 7 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 _ 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 7 6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 1 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 2 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 8 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 8 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 5 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 7 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 1 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 _ 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 7 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 _ 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 5 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_ 7 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 _ 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 5 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 8 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 3 _ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 8 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 1 5 </t>
-  </si>
-  <si>
-    <t>Mean</t>
-  </si>
-  <si>
-    <t>Median</t>
-  </si>
-  <si>
-    <t>Mode</t>
-  </si>
-  <si>
-    <t>StdDev</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Memory</t>
-  </si>
-  <si>
-    <t>Boards</t>
   </si>
 </sst>
 </file>
@@ -666,7 +654,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -935,11 +922,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-11516160"/>
-        <c:axId val="-12178464"/>
+        <c:axId val="62694496"/>
+        <c:axId val="65165472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-11516160"/>
+        <c:axId val="62694496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10.0"/>
@@ -986,7 +973,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1016,6 +1002,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1052,12 +1039,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-12178464"/>
+        <c:crossAx val="65165472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-12178464"/>
+        <c:axId val="65165472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1109,7 +1096,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1176,7 +1162,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-11516160"/>
+        <c:crossAx val="62694496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2081,7 +2067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -2107,13 +2093,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2391,13 +2377,13 @@
         <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="J18" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="K18" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -2417,7 +2403,7 @@
         <v>41225</v>
       </c>
       <c r="G19" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H19" s="3">
         <f>AVERAGE(B3:B32)</f>
@@ -2453,7 +2439,7 @@
         <v>63160</v>
       </c>
       <c r="G20" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H20" s="3">
         <f>MEDIAN(B3:B32)</f>
@@ -2489,7 +2475,7 @@
         <v>99659</v>
       </c>
       <c r="G21" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H21" s="3">
         <f>MODE(B3:B32)</f>
@@ -2516,7 +2502,7 @@
         <v>49480</v>
       </c>
       <c r="G22" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H22" s="3">
         <f>_xlfn.STDEV.S(B3:B32)</f>
@@ -2729,10 +2715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F123"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2759,1210 +2745,1190 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F7" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F9" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E12" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F13" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E17" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F17" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E19" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F19" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D20" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C21" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E21" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F21" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C23" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D23" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E23" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D24" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C25" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E25" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F25" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E27" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F27" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D28" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D29" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E29" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F29" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D31" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E31" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F31" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D32" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F32" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E33" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F33" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C35" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E35" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D36" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E36" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F36" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E37" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F37" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C39" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D39" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E39" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F39" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D40" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E40" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F40" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C41" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D41" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E41" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F41" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D43" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E43" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F43" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D44" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E44" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F44" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C45" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D45" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E45" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F45" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B47" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D47" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E47" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F47" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E48" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F48" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C49" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D49" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E49" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F49" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B51" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C51" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D51" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E51" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F51" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C52" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D52" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E52" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F52" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D53" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E53" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B55" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C55" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D55" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E55" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F55" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D56" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E56" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F56" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C57" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D57" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E57" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F57" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B59" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D59" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E59" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F59" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E60" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F60" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C61" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D61" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E61" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F61" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B63" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C63" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D63" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E63" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F63" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C64" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D64" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E64" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F64" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C65" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D65" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E65" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F65" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B67" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C67" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D67" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F67" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C68" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D68" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E68" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F68" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C69" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D69" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E69" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B71" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C71" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D71" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F71" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C72" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D72" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F72" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C73" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D73" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E73" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D75" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F75" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D76" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F76" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D77" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F77" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B79" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D79" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F79" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D80" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F80" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D81" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F81" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B83" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D83" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F83" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D84" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F84" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D85" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F85" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D87" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F87" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D88" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F88" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D89" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F89" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F91" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F92" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F93" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F95" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F96" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F97" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F99" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F100" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F101" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed BFS no CL code
</commit_message>
<xml_diff>
--- a/Project1/Project1/Project1.xlsx
+++ b/Project1/Project1/Project1.xlsx
@@ -9,11 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="27280" windowHeight="16260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="34280" yWindow="-240" windowWidth="28840" windowHeight="16260" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="BFS Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Final Data" sheetId="7" r:id="rId1"/>
+    <sheet name="BFS Data" sheetId="1" r:id="rId2"/>
+    <sheet name="BFS NoCL Data" sheetId="3" r:id="rId3"/>
+    <sheet name="DFS Data" sheetId="4" r:id="rId4"/>
+    <sheet name="ASTAR V1 Data" sheetId="5" r:id="rId5"/>
+    <sheet name="ASTAR V2 Data" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="180">
   <si>
     <t>BFS</t>
   </si>
@@ -550,6 +555,24 @@
   </si>
   <si>
     <t>SOLVED</t>
+  </si>
+  <si>
+    <t>BFS - No Closed List</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>BFS w/o Closed List</t>
+  </si>
+  <si>
+    <t>A* V1</t>
+  </si>
+  <si>
+    <t>A* V2</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
   </si>
 </sst>
 </file>
@@ -594,12 +617,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,6 +680,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -922,11 +949,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="62694496"/>
-        <c:axId val="65165472"/>
+        <c:axId val="61920608"/>
+        <c:axId val="60986880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="62694496"/>
+        <c:axId val="61920608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10.0"/>
@@ -973,6 +1000,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1039,12 +1067,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65165472"/>
+        <c:crossAx val="60986880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65165472"/>
+        <c:axId val="60986880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1096,6 +1124,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1162,7 +1191,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62694496"/>
+        <c:crossAx val="61920608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1771,16 +1800,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>762203</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>51003</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>122345</xdr:rowOff>
+      <xdr:rowOff>147745</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>313955</xdr:colOff>
+      <xdr:colOff>428255</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>63847</xdr:rowOff>
+      <xdr:rowOff>89247</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2065,10 +2094,387 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="3">
+        <f>'BFS Data'!H19</f>
+        <v>20.766666666666666</v>
+      </c>
+      <c r="C3" s="3" t="e">
+        <f>'BFS NoCL Data'!H19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D3" s="3" t="e">
+        <f>'DFS Data'!H19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E3" s="3" t="e">
+        <f>'ASTAR V1 Data'!H19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F3" s="3" t="e">
+        <f>'ASTAR V2 Data'!H19</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="3">
+        <f>'BFS Data'!H20</f>
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="e">
+        <f>'BFS NoCL Data'!H20</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D4" s="3" t="e">
+        <f>'DFS Data'!H20</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E4" s="3" t="e">
+        <f>'ASTAR V1 Data'!H20</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F4" s="3" t="e">
+        <f>'ASTAR V2 Data'!H20</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="3">
+        <f>'BFS Data'!H21</f>
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="e">
+        <f>'BFS NoCL Data'!H21</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D5" s="3" t="e">
+        <f>'DFS Data'!H21</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E5" s="3" t="e">
+        <f>'ASTAR V1 Data'!H21</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F5" s="3" t="e">
+        <f>'ASTAR V2 Data'!H21</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="3">
+        <f>'BFS Data'!H22</f>
+        <v>2.9790455927491553</v>
+      </c>
+      <c r="C6" s="3" t="e">
+        <f>'BFS NoCL Data'!H22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D6" s="3" t="e">
+        <f>'DFS Data'!H22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E6" s="3" t="e">
+        <f>'ASTAR V1 Data'!H22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F6" s="3" t="e">
+        <f>'ASTAR V2 Data'!H22</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9">
+        <f>'BFS Data'!I19</f>
+        <v>8.1963333333333352</v>
+      </c>
+      <c r="C9" s="3" t="e">
+        <f>'BFS NoCL Data'!I19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D9" s="3" t="e">
+        <f>'DFS Data'!I19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E9" s="3" t="e">
+        <f>'ASTAR V1 Data'!I19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F9" s="3" t="e">
+        <f>'ASTAR V2 Data'!I19</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10">
+        <f>'BFS Data'!I20</f>
+        <v>5.7650000000000006</v>
+      </c>
+      <c r="C10" s="3" t="e">
+        <f>'BFS NoCL Data'!I20</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D10" s="3" t="e">
+        <f>'DFS Data'!I20</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E10" s="3" t="e">
+        <f>'ASTAR V1 Data'!I20</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F10" s="3" t="e">
+        <f>'ASTAR V2 Data'!I20</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11">
+        <f>'BFS Data'!I22</f>
+        <v>7.3534423012736605</v>
+      </c>
+      <c r="C11" s="3" t="e">
+        <f>'BFS NoCL Data'!I22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D11" s="3" t="e">
+        <f>'DFS Data'!I22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" s="3" t="e">
+        <f>'ASTAR V1 Data'!I22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" s="3" t="e">
+        <f>'ASTAR V2 Data'!I22</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" s="3">
+        <f>'BFS Data'!J19</f>
+        <v>85.923333333333318</v>
+      </c>
+      <c r="C14" s="3" t="e">
+        <f>'BFS NoCL Data'!J19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D14" s="3" t="e">
+        <f>'DFS Data'!J19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E14" s="3" t="e">
+        <f>'ASTAR V1 Data'!J19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" s="3" t="e">
+        <f>'ASTAR V2 Data'!J19</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B15" s="3">
+        <f>'BFS Data'!J20</f>
+        <v>90.5</v>
+      </c>
+      <c r="C15" s="3" t="e">
+        <f>'BFS NoCL Data'!J20</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D15" s="3" t="e">
+        <f>'DFS Data'!J20</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E15" s="3" t="e">
+        <f>'ASTAR V1 Data'!J20</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F15" s="3" t="e">
+        <f>'ASTAR V2 Data'!J20</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B16" s="3">
+        <f>'BFS Data'!J22</f>
+        <v>34.322393246405824</v>
+      </c>
+      <c r="C16" s="3" t="e">
+        <f>'BFS NoCL Data'!J22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D16" s="3" t="e">
+        <f>'DFS Data'!J22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E16" s="3" t="e">
+        <f>'ASTAR V1 Data'!J22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" s="3" t="e">
+        <f>'ASTAR V2 Data'!J22</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" s="4">
+        <f>'BFS Data'!K19</f>
+        <v>72363.566666666666</v>
+      </c>
+      <c r="C19" s="3" t="e">
+        <f>'BFS NoCL Data'!K19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D19" s="3" t="e">
+        <f>'DFS Data'!K19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E19" s="3" t="e">
+        <f>'ASTAR V1 Data'!K19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F19" s="3" t="e">
+        <f>'ASTAR V2 Data'!K19</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="4">
+        <f>'BFS Data'!K20</f>
+        <v>66591</v>
+      </c>
+      <c r="C20" s="3" t="e">
+        <f>'BFS NoCL Data'!K20</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D20" s="3" t="e">
+        <f>'DFS Data'!K20</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E20" s="3" t="e">
+        <f>'ASTAR V1 Data'!K20</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F20" s="3" t="e">
+        <f>'ASTAR V2 Data'!K20</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21" s="4">
+        <f>'BFS Data'!K22</f>
+        <v>47568.043928151754</v>
+      </c>
+      <c r="C21" s="3" t="e">
+        <f>'BFS NoCL Data'!K22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D21" s="3" t="e">
+        <f>'DFS Data'!K22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E21" s="3" t="e">
+        <f>'ASTAR V1 Data'!K22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F21" s="3" t="e">
+        <f>'ASTAR V2 Data'!K22</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2713,12 +3119,1416 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="8" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="H18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>170</v>
+      </c>
+      <c r="J18" t="s">
+        <v>171</v>
+      </c>
+      <c r="K18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="G19" t="s">
+        <v>166</v>
+      </c>
+      <c r="H19" s="3" t="e">
+        <f>AVERAGE(B3:B32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="2" t="e">
+        <f t="shared" ref="I19:J19" si="0">AVERAGE(C3:C32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K19" s="4" t="e">
+        <f>AVERAGE(E3:E32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="G20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H20" s="3" t="e">
+        <f>MEDIAN(B3:B32)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="I20" s="3" t="e">
+        <f t="shared" ref="I20:K20" si="1">MEDIAN(C3:C32)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="J20" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K20" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="G21" t="s">
+        <v>168</v>
+      </c>
+      <c r="H21" s="3" t="e">
+        <f>MODE(B3:B32)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="G22" t="s">
+        <v>169</v>
+      </c>
+      <c r="H22" s="3" t="e">
+        <f>_xlfn.STDEV.S(B3:B32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="3" t="e">
+        <f>_xlfn.STDEV.S(C3:C32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22" s="3" t="e">
+        <f>_xlfn.STDEV.S(D3:D32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K22" s="4" t="e">
+        <f>_xlfn.STDEV.S(E3:E32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="8" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="H18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>170</v>
+      </c>
+      <c r="J18" t="s">
+        <v>171</v>
+      </c>
+      <c r="K18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="G19" t="s">
+        <v>166</v>
+      </c>
+      <c r="H19" s="3" t="e">
+        <f>AVERAGE(B3:B32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="2" t="e">
+        <f t="shared" ref="I19:J19" si="0">AVERAGE(C3:C32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K19" s="4" t="e">
+        <f>AVERAGE(E3:E32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="G20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H20" s="3" t="e">
+        <f>MEDIAN(B3:B32)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="I20" s="3" t="e">
+        <f t="shared" ref="I20:K20" si="1">MEDIAN(C3:C32)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="J20" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K20" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="G21" t="s">
+        <v>168</v>
+      </c>
+      <c r="H21" s="3" t="e">
+        <f>MODE(B3:B32)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="G22" t="s">
+        <v>169</v>
+      </c>
+      <c r="H22" s="3" t="e">
+        <f>_xlfn.STDEV.S(B3:B32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="3" t="e">
+        <f>_xlfn.STDEV.S(C3:C32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22" s="3" t="e">
+        <f>_xlfn.STDEV.S(D3:D32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K22" s="4" t="e">
+        <f>_xlfn.STDEV.S(E3:E32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="8" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="H18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>170</v>
+      </c>
+      <c r="J18" t="s">
+        <v>171</v>
+      </c>
+      <c r="K18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="G19" t="s">
+        <v>166</v>
+      </c>
+      <c r="H19" s="3" t="e">
+        <f>AVERAGE(B3:B32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="2" t="e">
+        <f t="shared" ref="I19:J19" si="0">AVERAGE(C3:C32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K19" s="4" t="e">
+        <f>AVERAGE(E3:E32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="G20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H20" s="3" t="e">
+        <f>MEDIAN(B3:B32)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="I20" s="3" t="e">
+        <f t="shared" ref="I20:K20" si="1">MEDIAN(C3:C32)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="J20" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K20" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="G21" t="s">
+        <v>168</v>
+      </c>
+      <c r="H21" s="3" t="e">
+        <f>MODE(B3:B32)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="G22" t="s">
+        <v>169</v>
+      </c>
+      <c r="H22" s="3" t="e">
+        <f>_xlfn.STDEV.S(B3:B32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="3" t="e">
+        <f>_xlfn.STDEV.S(C3:C32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22" s="3" t="e">
+        <f>_xlfn.STDEV.S(D3:D32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K22" s="4" t="e">
+        <f>_xlfn.STDEV.S(E3:E32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="8" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="H18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>170</v>
+      </c>
+      <c r="J18" t="s">
+        <v>171</v>
+      </c>
+      <c r="K18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="G19" t="s">
+        <v>166</v>
+      </c>
+      <c r="H19" s="3" t="e">
+        <f>AVERAGE(B3:B32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="2" t="e">
+        <f t="shared" ref="I19:J19" si="0">AVERAGE(C3:C32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K19" s="4" t="e">
+        <f>AVERAGE(E3:E32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="G20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H20" s="3" t="e">
+        <f>MEDIAN(B3:B32)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="I20" s="3" t="e">
+        <f t="shared" ref="I20:K20" si="1">MEDIAN(C3:C32)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="J20" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K20" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="G21" t="s">
+        <v>168</v>
+      </c>
+      <c r="H21" s="3" t="e">
+        <f>MODE(B3:B32)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="G22" t="s">
+        <v>169</v>
+      </c>
+      <c r="H22" s="3" t="e">
+        <f>_xlfn.STDEV.S(B3:B32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="3" t="e">
+        <f>_xlfn.STDEV.S(C3:C32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22" s="3" t="e">
+        <f>_xlfn.STDEV.S(D3:D32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K22" s="4" t="e">
+        <f>_xlfn.STDEV.S(E3:E32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed BFS NoCL checks
</commit_message>
<xml_diff>
--- a/Project1/Project1/Project1.xlsx
+++ b/Project1/Project1/Project1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34280" yWindow="-240" windowWidth="28840" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="22180" windowHeight="16220" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Final Data" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="DFS Data" sheetId="4" r:id="rId4"/>
     <sheet name="ASTAR V1 Data" sheetId="5" r:id="rId5"/>
     <sheet name="ASTAR V2 Data" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -579,10 +580,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -614,10 +623,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -626,8 +636,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -741,6 +753,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.200416016100273"/>
+                  <c:y val="0.054285931675748"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'BFS Data'!$B$3:$B$32</c:f>
@@ -748,94 +811,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>21.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25.0</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.0</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.0</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>25.0</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="18">
                   <c:v>21.0</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="19">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>20.0</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>18.0</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>25.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>19.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>22.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>20.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>21.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -847,94 +910,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>64750.0</c:v>
+                  <c:v>46144.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18503.0</c:v>
+                  <c:v>76318.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>94348.0</c:v>
+                  <c:v>124529.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21080.0</c:v>
+                  <c:v>29908.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>148181.0</c:v>
+                  <c:v>62004.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>101314.0</c:v>
+                  <c:v>178036.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>161612.0</c:v>
+                  <c:v>7471.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21874.0</c:v>
+                  <c:v>142050.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>60356.0</c:v>
+                  <c:v>87946.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90035.0</c:v>
+                  <c:v>98397.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>144870.0</c:v>
+                  <c:v>88450.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6585.0</c:v>
+                  <c:v>91754.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>73493.0</c:v>
+                  <c:v>83286.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>53307.0</c:v>
+                  <c:v>82327.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>158745.0</c:v>
+                  <c:v>1166.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>19292.0</c:v>
+                  <c:v>163174.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41225.0</c:v>
+                  <c:v>165086.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>63160.0</c:v>
+                  <c:v>151806.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>99659.0</c:v>
+                  <c:v>59939.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>49480.0</c:v>
+                  <c:v>25855.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>113560.0</c:v>
+                  <c:v>145490.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2116.0</c:v>
+                  <c:v>20037.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>72695.0</c:v>
+                  <c:v>8790.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>17986.0</c:v>
+                  <c:v>43750.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>150963.0</c:v>
+                  <c:v>119174.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>31488.0</c:v>
+                  <c:v>127313.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>104265.0</c:v>
+                  <c:v>75500.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>76072.0</c:v>
+                  <c:v>29980.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41461.0</c:v>
+                  <c:v>40295.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>68432.0</c:v>
+                  <c:v>34497.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -949,11 +1012,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61920608"/>
-        <c:axId val="60986880"/>
+        <c:axId val="529687488"/>
+        <c:axId val="529703488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61920608"/>
+        <c:axId val="529687488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10.0"/>
@@ -1067,12 +1130,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60986880"/>
+        <c:crossAx val="529703488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60986880"/>
+        <c:axId val="529703488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1191,7 +1254,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61920608"/>
+        <c:crossAx val="529687488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2096,7 +2159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -2130,7 +2193,7 @@
       </c>
       <c r="B3" s="3">
         <f>'BFS Data'!H19</f>
-        <v>20.766666666666666</v>
+        <v>21.266666666666666</v>
       </c>
       <c r="C3" s="3" t="e">
         <f>'BFS NoCL Data'!H19</f>
@@ -2155,7 +2218,7 @@
       </c>
       <c r="B4" s="3">
         <f>'BFS Data'!H20</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="e">
         <f>'BFS NoCL Data'!H20</f>
@@ -2180,7 +2243,7 @@
       </c>
       <c r="B5" s="3">
         <f>'BFS Data'!H21</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="e">
         <f>'BFS NoCL Data'!H21</f>
@@ -2205,7 +2268,7 @@
       </c>
       <c r="B6" s="3">
         <f>'BFS Data'!H22</f>
-        <v>2.9790455927491553</v>
+        <v>3.5712775009099684</v>
       </c>
       <c r="C6" s="3" t="e">
         <f>'BFS NoCL Data'!H22</f>
@@ -2235,7 +2298,7 @@
       </c>
       <c r="B9">
         <f>'BFS Data'!I19</f>
-        <v>8.1963333333333352</v>
+        <v>14.845333333333334</v>
       </c>
       <c r="C9" s="3" t="e">
         <f>'BFS NoCL Data'!I19</f>
@@ -2260,7 +2323,7 @@
       </c>
       <c r="B10">
         <f>'BFS Data'!I20</f>
-        <v>5.7650000000000006</v>
+        <v>14.015000000000001</v>
       </c>
       <c r="C10" s="3" t="e">
         <f>'BFS NoCL Data'!I20</f>
@@ -2285,7 +2348,7 @@
       </c>
       <c r="B11">
         <f>'BFS Data'!I22</f>
-        <v>7.3534423012736605</v>
+        <v>11.714037771816347</v>
       </c>
       <c r="C11" s="3" t="e">
         <f>'BFS NoCL Data'!I22</f>
@@ -2315,7 +2378,7 @@
       </c>
       <c r="B14" s="3">
         <f>'BFS Data'!J19</f>
-        <v>85.923333333333318</v>
+        <v>80.520000000000024</v>
       </c>
       <c r="C14" s="3" t="e">
         <f>'BFS NoCL Data'!J19</f>
@@ -2340,7 +2403,7 @@
       </c>
       <c r="B15" s="3">
         <f>'BFS Data'!J20</f>
-        <v>90.5</v>
+        <v>86.9</v>
       </c>
       <c r="C15" s="3" t="e">
         <f>'BFS NoCL Data'!J20</f>
@@ -2365,7 +2428,7 @@
       </c>
       <c r="B16" s="3">
         <f>'BFS Data'!J22</f>
-        <v>34.322393246405824</v>
+        <v>30.682291871415888</v>
       </c>
       <c r="C16" s="3" t="e">
         <f>'BFS NoCL Data'!J22</f>
@@ -2395,7 +2458,7 @@
       </c>
       <c r="B19" s="4">
         <f>'BFS Data'!K19</f>
-        <v>72363.566666666666</v>
+        <v>80349.066666666666</v>
       </c>
       <c r="C19" s="3" t="e">
         <f>'BFS NoCL Data'!K19</f>
@@ -2420,7 +2483,7 @@
       </c>
       <c r="B20" s="4">
         <f>'BFS Data'!K20</f>
-        <v>66591</v>
+        <v>79322.5</v>
       </c>
       <c r="C20" s="3" t="e">
         <f>'BFS NoCL Data'!K20</f>
@@ -2445,7 +2508,7 @@
       </c>
       <c r="B21" s="4">
         <f>'BFS Data'!K22</f>
-        <v>47568.043928151754</v>
+        <v>51993.196178182669</v>
       </c>
       <c r="C21" s="3" t="e">
         <f>'BFS NoCL Data'!K22</f>
@@ -2474,7 +2537,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2513,16 +2576,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>5.0599999999999996</v>
+        <v>5.69</v>
       </c>
       <c r="D3">
-        <v>95.4</v>
+        <v>63.5</v>
       </c>
       <c r="E3">
-        <v>64750</v>
+        <v>46144</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2530,16 +2593,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C4">
-        <v>0.86</v>
+        <v>11.29</v>
       </c>
       <c r="D4">
-        <v>47.9</v>
+        <v>84.3</v>
       </c>
       <c r="E4">
-        <v>18503</v>
+        <v>76318</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2547,16 +2610,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>8.81</v>
+        <v>20.190000000000001</v>
       </c>
       <c r="D5">
-        <v>116.4</v>
+        <v>109</v>
       </c>
       <c r="E5">
-        <v>94348</v>
+        <v>124529</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2564,16 +2627,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6">
-        <v>1.41</v>
+        <v>3.36</v>
       </c>
       <c r="D6">
-        <v>43.4</v>
+        <v>49.1</v>
       </c>
       <c r="E6">
-        <v>21080</v>
+        <v>29908</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2581,16 +2644,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>18.86</v>
+        <v>8.5</v>
       </c>
       <c r="D7">
-        <v>147</v>
+        <v>75.3</v>
       </c>
       <c r="E7">
-        <v>148181</v>
+        <v>62004</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2598,16 +2661,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C8">
-        <v>13.42</v>
+        <v>32.869999999999997</v>
       </c>
       <c r="D8">
-        <v>107.2</v>
+        <v>119</v>
       </c>
       <c r="E8">
-        <v>101314</v>
+        <v>178036</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2615,16 +2678,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>23.95</v>
+        <v>0.77</v>
       </c>
       <c r="D9">
-        <v>130.30000000000001</v>
+        <v>25.1</v>
       </c>
       <c r="E9">
-        <v>161612</v>
+        <v>7471</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2632,16 +2695,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C10">
-        <v>1.1000000000000001</v>
+        <v>24.32</v>
       </c>
       <c r="D10">
-        <v>44.8</v>
+        <v>115</v>
       </c>
       <c r="E10">
-        <v>21874</v>
+        <v>142050</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2649,16 +2712,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11">
-        <v>6.67</v>
+        <v>13.72</v>
       </c>
       <c r="D11">
-        <v>77.599999999999994</v>
+        <v>95.7</v>
       </c>
       <c r="E11">
-        <v>60356</v>
+        <v>87946</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2669,13 +2732,13 @@
         <v>22</v>
       </c>
       <c r="C12">
-        <v>10.38</v>
+        <v>16.48</v>
       </c>
       <c r="D12">
-        <v>103.4</v>
+        <v>101.2</v>
       </c>
       <c r="E12">
-        <v>90035</v>
+        <v>98397</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2683,16 +2746,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13">
-        <v>18.329999999999998</v>
+        <v>16.170000000000002</v>
       </c>
       <c r="D13">
-        <v>140</v>
+        <v>95.2</v>
       </c>
       <c r="E13">
-        <v>144870</v>
+        <v>88450</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2700,16 +2763,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C14">
-        <v>0.24</v>
+        <v>16.53</v>
       </c>
       <c r="D14">
-        <v>26.9</v>
+        <v>97.6</v>
       </c>
       <c r="E14">
-        <v>6585</v>
+        <v>91754</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2717,16 +2780,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15">
-        <v>8.08</v>
+        <v>14.37</v>
       </c>
       <c r="D15">
-        <v>90.9</v>
+        <v>90.8</v>
       </c>
       <c r="E15">
-        <v>73493</v>
+        <v>83286</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2734,16 +2797,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C16">
-        <v>3.65</v>
+        <v>14.79</v>
       </c>
       <c r="D16">
-        <v>85.6</v>
+        <v>89.5</v>
       </c>
       <c r="E16">
-        <v>53307</v>
+        <v>82327</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -2751,16 +2814,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C17">
-        <v>23.74</v>
+        <v>0.13</v>
       </c>
       <c r="D17">
-        <v>125.2</v>
+        <v>20.9</v>
       </c>
       <c r="E17">
-        <v>158745</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -2768,16 +2831,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="1">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1">
-        <v>1.3</v>
+        <v>35.35</v>
       </c>
       <c r="D18" s="1">
-        <v>41.8</v>
+        <v>117.5</v>
       </c>
       <c r="E18" s="1">
-        <v>19292</v>
+        <v>163174</v>
       </c>
       <c r="H18" t="s">
         <v>2</v>
@@ -2797,35 +2860,35 @@
         <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1">
-        <v>2.4900000000000002</v>
+        <v>39.53</v>
       </c>
       <c r="D19" s="1">
-        <v>67.8</v>
+        <v>117.6</v>
       </c>
       <c r="E19" s="1">
-        <v>41225</v>
+        <v>165086</v>
       </c>
       <c r="G19" t="s">
         <v>166</v>
       </c>
       <c r="H19" s="3">
         <f>AVERAGE(B3:B32)</f>
-        <v>20.766666666666666</v>
+        <v>21.266666666666666</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" ref="I19:J19" si="0">AVERAGE(C3:C32)</f>
-        <v>8.1963333333333352</v>
+        <v>14.845333333333334</v>
       </c>
       <c r="J19" s="3">
         <f t="shared" si="0"/>
-        <v>85.923333333333318</v>
+        <v>80.520000000000024</v>
       </c>
       <c r="K19" s="4">
         <f>AVERAGE(E3:E32)</f>
-        <v>72363.566666666666</v>
+        <v>80349.066666666666</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -2833,35 +2896,35 @@
         <v>18</v>
       </c>
       <c r="B20" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1">
-        <v>4.9400000000000004</v>
+        <v>35.69</v>
       </c>
       <c r="D20" s="1">
-        <v>85.6</v>
+        <v>115.4</v>
       </c>
       <c r="E20" s="1">
-        <v>63160</v>
+        <v>151806</v>
       </c>
       <c r="G20" t="s">
         <v>167</v>
       </c>
       <c r="H20" s="3">
         <f>MEDIAN(B3:B32)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I20" s="3">
         <f t="shared" ref="I20:K20" si="1">MEDIAN(C3:C32)</f>
-        <v>5.7650000000000006</v>
+        <v>14.015000000000001</v>
       </c>
       <c r="J20" s="3">
         <f t="shared" si="1"/>
-        <v>90.5</v>
+        <v>86.9</v>
       </c>
       <c r="K20" s="4">
         <f t="shared" si="1"/>
-        <v>66591</v>
+        <v>79322.5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -2869,23 +2932,23 @@
         <v>19</v>
       </c>
       <c r="B21" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="1">
-        <v>11.81</v>
+        <v>10.08</v>
       </c>
       <c r="D21" s="1">
-        <v>110.8</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="E21" s="1">
-        <v>99659</v>
+        <v>59939</v>
       </c>
       <c r="G21" t="s">
         <v>168</v>
       </c>
       <c r="H21" s="3">
         <f>MODE(B3:B32)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -2896,35 +2959,35 @@
         <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1">
-        <v>3.3</v>
+        <v>3.53</v>
       </c>
       <c r="D22" s="1">
-        <v>77.3</v>
+        <v>46.2</v>
       </c>
       <c r="E22" s="1">
-        <v>49480</v>
+        <v>25855</v>
       </c>
       <c r="G22" t="s">
         <v>169</v>
       </c>
       <c r="H22" s="3">
         <f>_xlfn.STDEV.S(B3:B32)</f>
-        <v>2.9790455927491553</v>
+        <v>3.5712775009099684</v>
       </c>
       <c r="I22" s="3">
         <f>_xlfn.STDEV.S(C3:C32)</f>
-        <v>7.3534423012736605</v>
+        <v>11.714037771816347</v>
       </c>
       <c r="J22" s="3">
         <f>_xlfn.STDEV.S(D3:D32)</f>
-        <v>34.322393246405824</v>
+        <v>30.682291871415888</v>
       </c>
       <c r="K22" s="4">
         <f>_xlfn.STDEV.S(E3:E32)</f>
-        <v>47568.043928151754</v>
+        <v>51993.196178182669</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -2932,16 +2995,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1">
-        <v>15.61</v>
+        <v>31.49</v>
       </c>
       <c r="D23" s="1">
-        <v>112.3</v>
+        <v>115.2</v>
       </c>
       <c r="E23" s="1">
-        <v>113560</v>
+        <v>145490</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -2949,16 +3012,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C24" s="1">
-        <v>0.2</v>
+        <v>2.62</v>
       </c>
       <c r="D24" s="1">
-        <v>21.3</v>
+        <v>40.5</v>
       </c>
       <c r="E24" s="1">
-        <v>2116</v>
+        <v>20037</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -2966,16 +3029,16 @@
         <v>23</v>
       </c>
       <c r="B25" s="1">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C25" s="1">
-        <v>6.05</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1">
-        <v>93.4</v>
+        <v>29.2</v>
       </c>
       <c r="E25" s="1">
-        <v>72695</v>
+        <v>8790</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -2983,16 +3046,16 @@
         <v>24</v>
       </c>
       <c r="B26" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C26" s="1">
-        <v>1.21</v>
+        <v>5.73</v>
       </c>
       <c r="D26" s="1">
-        <v>39.700000000000003</v>
+        <v>61.4</v>
       </c>
       <c r="E26" s="1">
-        <v>17986</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -3000,16 +3063,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="1">
-        <v>21.06</v>
+        <v>23.82</v>
       </c>
       <c r="D27" s="1">
-        <v>128.6</v>
+        <v>106.8</v>
       </c>
       <c r="E27" s="1">
-        <v>150963</v>
+        <v>119174</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -3017,16 +3080,16 @@
         <v>26</v>
       </c>
       <c r="B28" s="1">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C28" s="1">
-        <v>1.8</v>
+        <v>27.61</v>
       </c>
       <c r="D28" s="1">
-        <v>56.7</v>
+        <v>110.3</v>
       </c>
       <c r="E28" s="1">
-        <v>31488</v>
+        <v>127313</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -3037,13 +3100,13 @@
         <v>22</v>
       </c>
       <c r="C29" s="1">
-        <v>14.22</v>
+        <v>14.31</v>
       </c>
       <c r="D29" s="1">
-        <v>110.4</v>
+        <v>83.7</v>
       </c>
       <c r="E29" s="1">
-        <v>104265</v>
+        <v>75500</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -3051,16 +3114,16 @@
         <v>28</v>
       </c>
       <c r="B30" s="1">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C30" s="1">
-        <v>9.3000000000000007</v>
+        <v>4.3</v>
       </c>
       <c r="D30" s="1">
-        <v>90.1</v>
+        <v>48.8</v>
       </c>
       <c r="E30" s="1">
-        <v>76072</v>
+        <v>29980</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -3068,16 +3131,16 @@
         <v>29</v>
       </c>
       <c r="B31" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31" s="1">
-        <v>2.56</v>
+        <v>5.98</v>
       </c>
       <c r="D31" s="1">
-        <v>67.7</v>
+        <v>58.8</v>
       </c>
       <c r="E31" s="1">
-        <v>41461</v>
+        <v>40295</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -3085,16 +3148,16 @@
         <v>30</v>
       </c>
       <c r="B32" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C32" s="1">
-        <v>5.48</v>
+        <v>5.14</v>
       </c>
       <c r="D32" s="1">
-        <v>92.2</v>
+        <v>58.6</v>
       </c>
       <c r="E32" s="1">
-        <v>68432</v>
+        <v>34497</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -3112,7 +3175,7 @@
       <c r="E34" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -4525,6 +4588,585 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="32.5" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6">
+        <f>POWER(1.8,A1)</f>
+        <v>1.8</v>
+      </c>
+      <c r="C1" s="6">
+        <f>POWER(2,A1)</f>
+        <v>2</v>
+      </c>
+      <c r="D1" s="6">
+        <f>POWER(2.13,A1)</f>
+        <v>2.13</v>
+      </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <v>2</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6">
+        <f t="shared" ref="B2:B31" si="0">POWER(1.8,A2)</f>
+        <v>3.24</v>
+      </c>
+      <c r="C2" s="6">
+        <f t="shared" ref="C2:C31" si="1">POWER(2,A2)</f>
+        <v>4</v>
+      </c>
+      <c r="D2" s="6">
+        <f>POWER(2.13,A2)</f>
+        <v>4.5368999999999993</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6">
+        <f t="shared" si="0"/>
+        <v>5.8320000000000007</v>
+      </c>
+      <c r="C3" s="6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D3" s="6">
+        <f>POWER(2.13,A3)</f>
+        <v>9.6635969999999975</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <f t="shared" si="0"/>
+        <v>10.497600000000002</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="D4" s="6">
+        <f>POWER(2.13,A4)</f>
+        <v>20.583461609999993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6">
+        <f t="shared" si="0"/>
+        <v>18.895680000000006</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="D5" s="6">
+        <f>POWER(2.13,A5)</f>
+        <v>43.842773229299986</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6">
+        <f t="shared" si="0"/>
+        <v>34.01222400000001</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="D6" s="6">
+        <f>POWER(2.13,A6)</f>
+        <v>93.385106978408956</v>
+      </c>
+      <c r="I6">
+        <f>AVERAGE(F1:H3)</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6">
+        <f t="shared" si="0"/>
+        <v>61.222003200000017</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="D7" s="6">
+        <f>POWER(2.13,A7)</f>
+        <v>198.91027786401105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" si="0"/>
+        <v>110.19960576000004</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+      <c r="D8" s="6">
+        <f>POWER(2.13,A8)</f>
+        <v>423.67889185034352</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6">
+        <f t="shared" si="0"/>
+        <v>198.35929036800007</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" si="1"/>
+        <v>512</v>
+      </c>
+      <c r="D9" s="6">
+        <f>POWER(2.13,A9)</f>
+        <v>902.43603964123167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6">
+        <f t="shared" si="0"/>
+        <v>357.04672266240016</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" si="1"/>
+        <v>1024</v>
+      </c>
+      <c r="D10" s="6">
+        <f>POWER(2.13,A10)</f>
+        <v>1922.1887644358233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" s="6">
+        <f t="shared" si="0"/>
+        <v>642.68410079232035</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="1"/>
+        <v>2048</v>
+      </c>
+      <c r="D11" s="6">
+        <f>POWER(2.13,A11)</f>
+        <v>4094.262068248303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6">
+        <f t="shared" si="0"/>
+        <v>1156.8313814261767</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" si="1"/>
+        <v>4096</v>
+      </c>
+      <c r="D12" s="6">
+        <f>POWER(2.13,A12)</f>
+        <v>8720.7782053688843</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="6">
+        <f t="shared" si="0"/>
+        <v>2082.2964865671183</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="1"/>
+        <v>8192</v>
+      </c>
+      <c r="D13" s="6">
+        <f>POWER(2.13,A13)</f>
+        <v>18575.257577435725</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" s="6">
+        <f t="shared" si="0"/>
+        <v>3748.1336758208126</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="1"/>
+        <v>16384</v>
+      </c>
+      <c r="D14" s="6">
+        <f>POWER(2.13,A14)</f>
+        <v>39565.29863993809</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="6">
+        <f t="shared" si="0"/>
+        <v>6746.6406164774626</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="1"/>
+        <v>32768</v>
+      </c>
+      <c r="D15" s="6">
+        <f>POWER(2.13,A15)</f>
+        <v>84274.086103068112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" s="6">
+        <f t="shared" si="0"/>
+        <v>12143.953109659435</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="D16" s="6">
+        <f>POWER(2.13,A16)</f>
+        <v>179503.80339953507</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="6">
+        <f t="shared" si="0"/>
+        <v>21859.115597386983</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="1"/>
+        <v>131072</v>
+      </c>
+      <c r="D17" s="6">
+        <f>POWER(2.13,A17)</f>
+        <v>382343.10124100966</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" s="6">
+        <f t="shared" si="0"/>
+        <v>39346.408075296567</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" si="1"/>
+        <v>262144</v>
+      </c>
+      <c r="D18" s="6">
+        <f>POWER(2.13,A18)</f>
+        <v>814390.80564335058</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" s="6">
+        <f t="shared" si="0"/>
+        <v>70823.534535533836</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="1"/>
+        <v>524288</v>
+      </c>
+      <c r="D19" s="6">
+        <f>POWER(2.13,A19)</f>
+        <v>1734652.4160203366</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" s="6">
+        <f t="shared" si="0"/>
+        <v>127482.3621639609</v>
+      </c>
+      <c r="C20" s="6">
+        <f t="shared" si="1"/>
+        <v>1048576</v>
+      </c>
+      <c r="D20" s="6">
+        <f>POWER(2.13,A20)</f>
+        <v>3694809.6461233166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" s="6">
+        <f t="shared" si="0"/>
+        <v>229468.25189512965</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="1"/>
+        <v>2097152</v>
+      </c>
+      <c r="D21" s="6">
+        <f>POWER(2.13,A21)</f>
+        <v>7869944.5462426636</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" s="6">
+        <f t="shared" si="0"/>
+        <v>413042.8534112334</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="1"/>
+        <v>4194304</v>
+      </c>
+      <c r="D22" s="6">
+        <f>POWER(2.13,A22)</f>
+        <v>16762981.883496871</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" s="6">
+        <f t="shared" si="0"/>
+        <v>743477.1361402201</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" si="1"/>
+        <v>8388608</v>
+      </c>
+      <c r="D23" s="6">
+        <f>POWER(2.13,A23)</f>
+        <v>35705151.411848329</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" s="6">
+        <f t="shared" si="0"/>
+        <v>1338258.8450523962</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" si="1"/>
+        <v>16777216</v>
+      </c>
+      <c r="D24" s="6">
+        <f>POWER(2.13,A24)</f>
+        <v>76051972.507236943</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" s="6">
+        <f t="shared" si="0"/>
+        <v>2408865.9210943133</v>
+      </c>
+      <c r="C25" s="6">
+        <f t="shared" si="1"/>
+        <v>33554432</v>
+      </c>
+      <c r="D25" s="6">
+        <f>POWER(2.13,A25)</f>
+        <v>161990701.4404147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" s="6">
+        <f t="shared" si="0"/>
+        <v>4335958.6579697644</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" si="1"/>
+        <v>67108864</v>
+      </c>
+      <c r="D26" s="6">
+        <f>POWER(2.13,A26)</f>
+        <v>345040194.06808323</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" s="6">
+        <f t="shared" si="0"/>
+        <v>7804725.5843455764</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" si="1"/>
+        <v>134217728</v>
+      </c>
+      <c r="D27" s="6">
+        <f>POWER(2.13,A27)</f>
+        <v>734935613.36501718</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" s="6">
+        <f t="shared" si="0"/>
+        <v>14048506.051822038</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="1"/>
+        <v>268435456</v>
+      </c>
+      <c r="D28" s="6">
+        <f>POWER(2.13,A28)</f>
+        <v>1565412856.4674864</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" s="6">
+        <f t="shared" si="0"/>
+        <v>25287310.893279672</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="1"/>
+        <v>536870912</v>
+      </c>
+      <c r="D29" s="6">
+        <f>POWER(2.13,A29)</f>
+        <v>3334329384.2757463</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" s="6">
+        <f t="shared" si="0"/>
+        <v>45517159.607903406</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="1"/>
+        <v>1073741824</v>
+      </c>
+      <c r="D30" s="6">
+        <f>POWER(2.13,A30)</f>
+        <v>7102121588.5073395</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" s="6">
+        <f t="shared" si="0"/>
+        <v>81930887.294226125</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="1"/>
+        <v>2147483648</v>
+      </c>
+      <c r="D31" s="6">
+        <f>POWER(2.13,A31)</f>
+        <v>15127518983.52063</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5742,7 +6384,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Attempt to speed up A* Priority Queue
</commit_message>
<xml_diff>
--- a/Project1/Project1/Project1.xlsx
+++ b/Project1/Project1/Project1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38820" yWindow="-2060" windowWidth="24360" windowHeight="16220" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="5120" yWindow="2900" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Final Data" sheetId="7" r:id="rId1"/>
@@ -778,13 +778,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -842,7 +842,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -993,10 +992,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Final Data'!$B$6:$F$6</c:f>
+                <c:f>'Final Data'!$B$6:$G$6</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="6"/>
                   <c:pt idx="0">
                     <c:v>3.571277500909968</c:v>
                   </c:pt>
@@ -1012,15 +1011,18 @@
                   <c:pt idx="4">
                     <c:v>3.526582142697853</c:v>
                   </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.77509516267317</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Final Data'!$B$6:$F$6</c:f>
+                <c:f>'Final Data'!$B$6:$G$6</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="6"/>
                   <c:pt idx="0">
                     <c:v>3.571277500909968</c:v>
                   </c:pt>
@@ -1035,6 +1037,9 @@
                   </c:pt>
                   <c:pt idx="4">
                     <c:v>3.526582142697853</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.77509516267317</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1117,11 +1122,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="165012592"/>
-        <c:axId val="165014912"/>
+        <c:axId val="122240432"/>
+        <c:axId val="122269840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="165012592"/>
+        <c:axId val="122240432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1164,7 +1169,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165014912"/>
+        <c:crossAx val="122269840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1172,7 +1177,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165014912"/>
+        <c:axId val="122269840"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1224,7 +1229,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165012592"/>
+        <c:crossAx val="122240432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1316,7 +1321,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1418,11 +1422,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="249763632"/>
-        <c:axId val="248263520"/>
+        <c:axId val="275753856"/>
+        <c:axId val="269277328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="249763632"/>
+        <c:axId val="275753856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1465,7 +1469,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248263520"/>
+        <c:crossAx val="269277328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1473,7 +1477,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="248263520"/>
+        <c:axId val="269277328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1523,7 +1527,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249763632"/>
+        <c:crossAx val="275753856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1614,7 +1618,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1716,11 +1719,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="275306064"/>
-        <c:axId val="164844432"/>
+        <c:axId val="275638640"/>
+        <c:axId val="165248064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="275306064"/>
+        <c:axId val="275638640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1763,7 +1766,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164844432"/>
+        <c:crossAx val="165248064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1771,7 +1774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164844432"/>
+        <c:axId val="165248064"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1822,7 +1825,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275306064"/>
+        <c:crossAx val="275638640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1911,7 +1914,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2230,11 +2232,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="216216112"/>
-        <c:axId val="216219872"/>
+        <c:axId val="164750464"/>
+        <c:axId val="165309280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="216216112"/>
+        <c:axId val="164750464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10.0"/>
@@ -2281,7 +2283,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2348,12 +2349,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216219872"/>
+        <c:crossAx val="165309280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="216219872"/>
+        <c:axId val="165309280"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2407,7 +2408,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2474,7 +2474,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216216112"/>
+        <c:crossAx val="164750464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2856,11 +2856,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="216262656"/>
-        <c:axId val="216265136"/>
+        <c:axId val="274820528"/>
+        <c:axId val="165468288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="216262656"/>
+        <c:axId val="274820528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
@@ -2918,12 +2918,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216265136"/>
+        <c:crossAx val="165468288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="216265136"/>
+        <c:axId val="165468288"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2981,7 +2981,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216262656"/>
+        <c:crossAx val="274820528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3045,7 +3045,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3375,11 +3374,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="216293472"/>
-        <c:axId val="216295952"/>
+        <c:axId val="274765200"/>
+        <c:axId val="274767520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="216293472"/>
+        <c:axId val="274765200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3435,12 +3434,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216295952"/>
+        <c:crossAx val="274767520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="216295952"/>
+        <c:axId val="274767520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3496,7 +3495,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216293472"/>
+        <c:crossAx val="274765200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3560,7 +3559,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3890,11 +3888,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="271131712"/>
-        <c:axId val="302726976"/>
+        <c:axId val="275191552"/>
+        <c:axId val="275193600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="271131712"/>
+        <c:axId val="275191552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -3952,12 +3950,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302726976"/>
+        <c:crossAx val="275193600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="302726976"/>
+        <c:axId val="275193600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4013,7 +4011,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="271131712"/>
+        <c:crossAx val="275191552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4365,11 +4363,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276686224"/>
-        <c:axId val="275888224"/>
+        <c:axId val="274915872"/>
+        <c:axId val="269451856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276686224"/>
+        <c:axId val="274915872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4425,12 +4423,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275888224"/>
+        <c:crossAx val="269451856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="275888224"/>
+        <c:axId val="269451856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4486,7 +4484,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276686224"/>
+        <c:crossAx val="274915872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4838,11 +4836,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="275510800"/>
-        <c:axId val="275642528"/>
+        <c:axId val="270270160"/>
+        <c:axId val="250521408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="275510800"/>
+        <c:axId val="270270160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15.0"/>
@@ -4899,12 +4897,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275642528"/>
+        <c:crossAx val="250521408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="275642528"/>
+        <c:axId val="250521408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4960,7 +4958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275510800"/>
+        <c:crossAx val="270270160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5053,7 +5051,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6571,8 +6568,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.750841611740276"/>
-                  <c:y val="0.538641218279592"/>
+                  <c:x val="0.751391994986394"/>
+                  <c:y val="0.575027510579409"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -6813,11 +6810,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="217291520"/>
-        <c:axId val="217293296"/>
+        <c:axId val="122519456"/>
+        <c:axId val="122522000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="217291520"/>
+        <c:axId val="122519456"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -6871,7 +6868,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6901,6 +6897,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6937,12 +6934,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217293296"/>
+        <c:crossAx val="122522000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="217293296"/>
+        <c:axId val="122522000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="750000.0"/>
@@ -6990,7 +6987,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7057,7 +7053,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217291520"/>
+        <c:crossAx val="122519456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7071,7 +7067,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7182,7 +7177,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8942,11 +8936,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="217335712"/>
-        <c:axId val="217337504"/>
+        <c:axId val="270120912"/>
+        <c:axId val="249600240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="217335712"/>
+        <c:axId val="270120912"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -9005,12 +8999,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217337504"/>
+        <c:crossAx val="249600240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="217337504"/>
+        <c:axId val="249600240"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -9068,7 +9062,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217335712"/>
+        <c:crossAx val="270120912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9082,7 +9076,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9196,7 +9189,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9310,11 +9302,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="217351552"/>
-        <c:axId val="217354304"/>
+        <c:axId val="-117402640"/>
+        <c:axId val="-117400320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="217351552"/>
+        <c:axId val="-117402640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9357,7 +9349,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217354304"/>
+        <c:crossAx val="-117400320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9365,7 +9357,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217354304"/>
+        <c:axId val="-117400320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="760000.0"/>
@@ -9417,7 +9409,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217351552"/>
+        <c:crossAx val="-117402640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9509,7 +9501,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9623,11 +9614,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="217381008"/>
-        <c:axId val="217383760"/>
+        <c:axId val="-117375504"/>
+        <c:axId val="-117373184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="217381008"/>
+        <c:axId val="-117375504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9670,7 +9661,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217383760"/>
+        <c:crossAx val="-117373184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9678,7 +9669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217383760"/>
+        <c:axId val="-117373184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9728,7 +9719,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217381008"/>
+        <c:crossAx val="-117375504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9820,7 +9811,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9934,11 +9924,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="217403120"/>
-        <c:axId val="217405872"/>
+        <c:axId val="-116472672"/>
+        <c:axId val="-116470352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="217403120"/>
+        <c:axId val="-116472672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9981,7 +9971,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217405872"/>
+        <c:crossAx val="-116470352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9989,7 +9979,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217405872"/>
+        <c:axId val="-116470352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1900.0"/>
@@ -10041,7 +10031,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217403120"/>
+        <c:crossAx val="-116472672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10134,7 +10124,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10217,44 +10206,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.108198022949446"/>
-                  <c:y val="-0.0493620756793527"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -10503,44 +10456,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="exp"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.23544841419245"/>
-                  <c:y val="-0.0507772754518712"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -10789,44 +10706,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="exp"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.217631743240373"/>
-                  <c:y val="0.0540544448758466"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -11075,44 +10956,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="exp"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.0608918205624216"/>
-                  <c:y val="0.0793399576750041"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -11322,11 +11167,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="162858592"/>
-        <c:axId val="162862496"/>
+        <c:axId val="-116420624"/>
+        <c:axId val="-116417232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="162858592"/>
+        <c:axId val="-116420624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10.0"/>
@@ -11378,7 +11223,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11444,12 +11288,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162862496"/>
+        <c:crossAx val="-116417232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="162862496"/>
+        <c:axId val="-116417232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11495,7 +11339,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11562,7 +11405,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162858592"/>
+        <c:crossAx val="-116420624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11576,7 +11419,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11687,7 +11529,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12875,11 +12716,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="274831888"/>
-        <c:axId val="248851888"/>
+        <c:axId val="164766656"/>
+        <c:axId val="275013936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="274831888"/>
+        <c:axId val="164766656"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -12902,6 +12743,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -12938,12 +12780,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248851888"/>
+        <c:crossAx val="275013936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="248851888"/>
+        <c:axId val="275013936"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -13001,7 +12843,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274831888"/>
+        <c:crossAx val="164766656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13015,7 +12857,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13129,7 +12970,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13231,11 +13071,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="275856576"/>
-        <c:axId val="216877280"/>
+        <c:axId val="275530064"/>
+        <c:axId val="275367728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="275856576"/>
+        <c:axId val="275530064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13278,7 +13118,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216877280"/>
+        <c:crossAx val="275367728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13286,7 +13126,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216877280"/>
+        <c:axId val="275367728"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -13338,7 +13178,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275856576"/>
+        <c:crossAx val="275530064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23580,8 +23420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="C52" zoomScale="106" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23593,7 +23433,7 @@
     <col min="7" max="7" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -23642,7 +23482,7 @@
         <f>'ASTAR V2 Data'!H19</f>
         <v>19.333333333333332</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="14">
         <f>'Iterative Deepening'!H19</f>
         <v>25.6</v>
       </c>
@@ -23671,7 +23511,7 @@
         <f>'ASTAR V2 Data'!H20</f>
         <v>20.5</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="14">
         <f>'Iterative Deepening'!H20</f>
         <v>25.5</v>
       </c>
@@ -23700,7 +23540,7 @@
         <f>'ASTAR V2 Data'!H21</f>
         <v>22</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="14">
         <f>'Iterative Deepening'!H21</f>
         <v>25</v>
       </c>
@@ -23729,7 +23569,7 @@
         <f>'ASTAR V2 Data'!H22</f>
         <v>3.5265821426978534</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="14">
         <f>'Iterative Deepening'!H22</f>
         <v>5.7750951626731712</v>
       </c>
@@ -23775,7 +23615,7 @@
         <f>'ASTAR V2 Data'!I19</f>
         <v>0.27099999999999991</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="14">
         <f>'Iterative Deepening'!I19</f>
         <v>13.46</v>
       </c>
@@ -23804,7 +23644,7 @@
         <f>'ASTAR V2 Data'!I20</f>
         <v>0.11499999999999999</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="14">
         <f>'Iterative Deepening'!I20</f>
         <v>11.13</v>
       </c>
@@ -23833,7 +23673,7 @@
         <f>'ASTAR V2 Data'!I22</f>
         <v>0.33418299756580827</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="14">
         <f>'Iterative Deepening'!I22</f>
         <v>7.909446883316174</v>
       </c>
@@ -23879,7 +23719,7 @@
         <f>'ASTAR V2 Data'!J19</f>
         <v>20.963333333333335</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="14">
         <f>'Iterative Deepening'!J19</f>
         <v>28.266666666666669</v>
       </c>
@@ -23908,7 +23748,7 @@
         <f>'ASTAR V2 Data'!J20</f>
         <v>20.6</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="14">
         <f>'Iterative Deepening'!J20</f>
         <v>27.1</v>
       </c>
@@ -23937,7 +23777,7 @@
         <f>'ASTAR V2 Data'!J22</f>
         <v>0.83231431949521451</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="14">
         <f>'Iterative Deepening'!J22</f>
         <v>6.102816383940425</v>
       </c>
@@ -24731,10 +24571,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -25421,10 +25261,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -26073,10 +25913,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -26711,8 +26551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26725,10 +26565,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -27363,7 +27203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="125" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -27377,10 +27217,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">

</xml_diff>